<commit_message>
Added voxel percentages to Excel.
</commit_message>
<xml_diff>
--- a/Figures/Voxels_in_Yeo_networks.xlsx
+++ b/Figures/Voxels_in_Yeo_networks.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="14340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table_for_presentations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Network (Yeo)</t>
   </si>
@@ -34,13 +35,106 @@
   </si>
   <si>
     <t>When overlay the two in MRIcron, this seems plausible.</t>
+  </si>
+  <si>
+    <t>(In covaried model cluster composite mask, after reslicing Yeo network image to 4x4)</t>
+  </si>
+  <si>
+    <t>Frontal Pole</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule</t>
+  </si>
+  <si>
+    <t>Angular Gyrus</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex)</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex</t>
+  </si>
+  <si>
+    <t>Areas in Clust_Composite_Mask from Harvard-Oxford Atlas (atlasquery, probability of the mask being a member of the differently labeled regions in atlas)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Percentages</t>
+  </si>
+  <si>
+    <t>In resliced covaried model cluster composite mask multiplied by Yeo networks (network image first)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t># voxels</t>
+  </si>
+  <si>
+    <t>% of total cluster</t>
+  </si>
+  <si>
+    <t>Visual</t>
+  </si>
+  <si>
+    <t>Somatomotor</t>
+  </si>
+  <si>
+    <t>Dorsal Attention</t>
+  </si>
+  <si>
+    <t>Ventral Attention</t>
+  </si>
+  <si>
+    <t>Limbic</t>
+  </si>
+  <si>
+    <t>Frontoparietal</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -56,16 +150,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,15 +189,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,95 +586,581 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="60">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="3">
+        <f>(B2/529)*100</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <f>(F2/33643)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>217</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C9" si="0">(B3/529)*100</f>
+        <v>41.02079395085066</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>13808</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G9" si="1">(F3/33643)*100</f>
+        <v>41.042713194423804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3780718336483932</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>159</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.47260945813393568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>21.361058601134218</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>6852</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="1"/>
+        <v>20.366792497696402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5122873345935728</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>655</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9469131765894838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>4.536862003780719</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1628</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="1"/>
+        <v>4.8390452694468387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>165</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>31.190926275992435</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>10541</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="1"/>
+        <v>31.331926403709538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>529</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SUM(F2:F8)</f>
+        <v>33643</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="B11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:8">
       <c r="B12" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18">
+        <v>216</v>
+      </c>
+      <c r="C18">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19">
+        <v>207</v>
+      </c>
+      <c r="C19">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20">
+        <v>91</v>
+      </c>
+      <c r="C20">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21">
+        <v>105</v>
+      </c>
+      <c r="C21">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3.0013399999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>2.20932</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4.3222800000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>2.2595200000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>8.7404800000000005E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>2.6893799999999999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>5.5132199999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="2">
+        <v>4.6822100000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="2">
+        <v>6.1595700000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>1.1707799999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="2">
+        <v>19.8687</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="2">
+        <v>18.748100000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="2">
+        <v>5.6759300000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39">
+        <v>1.2366699999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>4.4822899999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31" thickBot="1">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" thickTop="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <f>(C2/529)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>217</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D9" si="0">(C3/529)*100</f>
+        <v>41.02079395085066</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.3780718336483932</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>113</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>21.361058601134218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5122873345935728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>4.536862003780719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>165</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>31.190926275992435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
+        <v>529</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="D10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>